<commit_message>
added one peptide's distance calculation
</commit_message>
<xml_diff>
--- a/Paths Example.xlsx
+++ b/Paths Example.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jraysajulga/Github/functional-tools-project/functional-tools-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE069C5-074A-B244-9231-1FE374BD0C47}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B488D607-DE6B-B049-918E-6574022C951A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10440" yWindow="7580" windowWidth="27640" windowHeight="16940" xr2:uid="{6302D645-88A4-D841-BB43-E692A16826A6}"/>
+    <workbookView xWindow="19860" yWindow="6980" windowWidth="31000" windowHeight="23500" activeTab="1" xr2:uid="{6302D645-88A4-D841-BB43-E692A16826A6}"/>
   </bookViews>
   <sheets>
     <sheet name="EEVAEEAQSGGD" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
   <si>
     <t>GO:0015630</t>
   </si>
@@ -250,13 +251,58 @@
   </si>
   <si>
     <t>GO:0019226(2);GO:0050877(1)</t>
+  </si>
+  <si>
+    <t>LCMGSGLNLCEPNNK</t>
+  </si>
+  <si>
+    <t>EggNOG Mapper</t>
+  </si>
+  <si>
+    <t>Ancestors</t>
+  </si>
+  <si>
+    <t>UniProtKB</t>
+  </si>
+  <si>
+    <t>Ancestors'kids</t>
+  </si>
+  <si>
+    <t>UniprotKB</t>
+  </si>
+  <si>
+    <t>descendants</t>
+  </si>
+  <si>
+    <t>MetaGOmics</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>UniProtKB to Ancestors</t>
+  </si>
+  <si>
+    <t>Extraneous to Ancestors' Kids</t>
+  </si>
+  <si>
+    <t>Extraneous to Ancestors</t>
+  </si>
+  <si>
+    <t>UniProtKB to Descendants</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -275,6 +321,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Sans"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -298,10 +350,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -317,6 +376,1027 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EggNOG Mapper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$D$6:$G$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>UniProtKB to Ancestors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Extraneous to Ancestors' Kids</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Extraneous to Ancestors</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UniProtKB to Descendants</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.97153</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.821429</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.573248</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E251-474A-AA9B-E68523FCAF09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MetaGOmics</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$D$6:$G$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>UniProtKB to Ancestors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Extraneous to Ancestors' Kids</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Extraneous to Ancestors</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>UniProtKB to Descendants</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$18:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.640523</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E251-474A-AA9B-E68523FCAF09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="835719600"/>
+        <c:axId val="888021952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="835719600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="888021952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="888021952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="835719600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3DF1CC2-CE5F-CA42-AF27-DB51DD01F9D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="406400"/>
+          <a:ext cx="7442200" cy="749300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8F6AEAD-142E-8442-B0AF-3750D8609FF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8280400" y="1892300"/>
+          <a:ext cx="7302500" cy="698500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1022350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{710E302E-F664-EB4F-874B-200E9ECCBD6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -618,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4835B2-FA6C-8044-A283-33BAE241C137}">
   <dimension ref="A2:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1225,4 +2305,170 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1072B7D7-74A4-5742-89AA-1F151F1DA92F}">
+  <dimension ref="A3:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="164" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="29.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7">
+        <v>3.97153</v>
+      </c>
+      <c r="E7">
+        <v>1.821429</v>
+      </c>
+      <c r="F7" s="5">
+        <v>3.573248</v>
+      </c>
+      <c r="G7">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8">
+        <v>0.83349640000000003</v>
+      </c>
+      <c r="F8">
+        <v>1.168798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9">
+        <v>1680</v>
+      </c>
+      <c r="F9">
+        <v>3140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3.640523</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ran through 6 more peptides
</commit_message>
<xml_diff>
--- a/Paths Example.xlsx
+++ b/Paths Example.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jraysajulga/Github/functional-tools-project/functional-tools-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B488D607-DE6B-B049-918E-6574022C951A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B8E844-A399-0C4B-8E39-FC09A8B2B341}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19860" yWindow="6980" windowWidth="31000" windowHeight="23500" activeTab="1" xr2:uid="{6302D645-88A4-D841-BB43-E692A16826A6}"/>
+    <workbookView xWindow="7900" yWindow="19620" windowWidth="25080" windowHeight="15540" activeTab="1" xr2:uid="{6302D645-88A4-D841-BB43-E692A16826A6}"/>
   </bookViews>
   <sheets>
     <sheet name="EEVAEEAQSGGD" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="100">
   <si>
     <t>GO:0015630</t>
   </si>
@@ -259,21 +260,6 @@
     <t>EggNOG Mapper</t>
   </si>
   <si>
-    <t>Ancestors</t>
-  </si>
-  <si>
-    <t>UniProtKB</t>
-  </si>
-  <si>
-    <t>Ancestors'kids</t>
-  </si>
-  <si>
-    <t>UniprotKB</t>
-  </si>
-  <si>
-    <t>descendants</t>
-  </si>
-  <si>
     <t>MetaGOmics</t>
   </si>
   <si>
@@ -296,13 +282,58 @@
   </si>
   <si>
     <t>UniProtKB to Descendants</t>
+  </si>
+  <si>
+    <t>FSPENTRK</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>EGTCPEAPTDECKPVK</t>
+  </si>
+  <si>
+    <t>RYIETDPANRDR</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>HVVPNEVVVQR</t>
+  </si>
+  <si>
+    <t>SCHLAMAPNHAVVSR</t>
+  </si>
+  <si>
+    <t>TPSLPTPPTREPK</t>
+  </si>
+  <si>
+    <t>LVRPEVDVMCTAFHDNEETFLK</t>
+  </si>
+  <si>
+    <t>IMCEILSSLQIGDFLVK</t>
+  </si>
+  <si>
+    <t>SCHLAMAPN</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>SIGHTPADAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -329,6 +360,25 @@
       <name val="Lucida Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFB0B0B0"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -350,17 +400,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,7 +460,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$7</c:f>
+              <c:f>Sheet2!$P$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -425,7 +481,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$D$6:$G$6</c:f>
+              <c:f>Sheet2!$C$6:$F$6</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -445,7 +501,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$7:$G$7</c:f>
+              <c:f>Sheet2!$Q$7:$T$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -475,7 +531,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$18</c:f>
+              <c:f>Sheet2!$V$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -496,7 +552,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$D$6:$G$6</c:f>
+              <c:f>Sheet2!$C$6:$F$6</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -516,18 +572,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$18:$G$18</c:f>
+              <c:f>Sheet2!$W$7:$Z$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3.640523</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
+                <c:pt idx="1">
+                  <c:v>2.3813230000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>1.1183540000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1274,16 +1330,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>604157</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>611414</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>34471</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1306,8 +1362,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7429500" y="406400"/>
-          <a:ext cx="7442200" cy="749300"/>
+          <a:off x="14066157" y="6600371"/>
+          <a:ext cx="7436757" cy="749300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1318,16 +1374,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>591457</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>85271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>459014</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>174171</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1350,8 +1406,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8280400" y="1892300"/>
-          <a:ext cx="7302500" cy="698500"/>
+          <a:off x="13227957" y="8213271"/>
+          <a:ext cx="7297057" cy="698500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1362,16 +1418,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1022350</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>664273</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>51552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266635</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171294</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1394,6 +1450,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>713508</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE0E05A-0C34-1947-B30B-53A27FE0669D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10873508" y="4267200"/>
+          <a:ext cx="4658591" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2309,166 +2409,1033 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1072B7D7-74A4-5742-89AA-1F151F1DA92F}">
-  <dimension ref="A3:G18"/>
+  <dimension ref="A4:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="164" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="1" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D3" s="4" t="s">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="C5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:26" ht="64" x14ac:dyDescent="0.2">
+      <c r="C6" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>75</v>
       </c>
       <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.4285709999999998</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3.573248</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2.5714290000000002</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2.9166669999999999</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4.1355930000000001</v>
+      </c>
+      <c r="P7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q7">
+        <v>3.97153</v>
+      </c>
+      <c r="R7">
+        <v>1.821429</v>
+      </c>
+      <c r="S7" s="4">
+        <v>3.573248</v>
+      </c>
+      <c r="T7">
+        <v>1.75</v>
+      </c>
+      <c r="U7" t="s">
+        <v>79</v>
+      </c>
+      <c r="V7" t="s">
+        <v>77</v>
+      </c>
+      <c r="W7" s="4">
+        <v>3.640523</v>
+      </c>
+      <c r="X7">
+        <v>2.3813230000000001</v>
+      </c>
+      <c r="Z7">
+        <v>1.1183540000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.3327850000000001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.283881</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.1723509999999999</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.245816</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.470755</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.3952830000000001</v>
+      </c>
+      <c r="R8">
+        <v>0.83349640000000003</v>
+      </c>
+      <c r="S8">
+        <v>1.168798</v>
+      </c>
+      <c r="U8" t="s">
+        <v>80</v>
+      </c>
+      <c r="X8">
+        <v>1.1944520000000001</v>
+      </c>
+      <c r="Z8">
+        <v>2.0967739999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="2">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2">
+        <v>157</v>
+      </c>
+      <c r="G9" s="2">
+        <v>119</v>
+      </c>
+      <c r="H9" s="2">
+        <v>48</v>
+      </c>
+      <c r="I9" s="2">
+        <v>59</v>
+      </c>
+      <c r="R9">
+        <v>1680</v>
+      </c>
+      <c r="S9">
+        <v>3140</v>
+      </c>
+      <c r="U9" t="s">
+        <v>78</v>
+      </c>
+      <c r="X9">
+        <v>10280</v>
+      </c>
+      <c r="Z9">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2.5714290000000002</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2.9166669999999999</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4.1355930000000001</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.245816</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.470755</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1.3952830000000001</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="2">
+        <v>119</v>
+      </c>
+      <c r="H12" s="2">
+        <v>48</v>
+      </c>
+      <c r="I12" s="2">
+        <v>59</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3.97153</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.8214286</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3.573248</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3.640523</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2.3813230000000001</v>
+      </c>
+      <c r="I16" s="2">
+        <v>3.940318</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2.0967739999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2.0786090000000002</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.83825280000000002</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1.1723509999999999</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.164965</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.9623569999999999</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.1955579999999999</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.345059</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1.1359239999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="2">
+        <v>281</v>
+      </c>
+      <c r="D18" s="2">
         <v>84</v>
       </c>
-      <c r="C7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7">
-        <v>3.97153</v>
-      </c>
-      <c r="E7">
-        <v>1.821429</v>
-      </c>
-      <c r="F7" s="5">
-        <v>3.573248</v>
-      </c>
-      <c r="G7">
+      <c r="E18" s="2">
+        <v>157</v>
+      </c>
+      <c r="F18" s="2">
+        <v>8</v>
+      </c>
+      <c r="G18" s="2">
+        <v>459</v>
+      </c>
+      <c r="H18" s="2">
+        <v>514</v>
+      </c>
+      <c r="I18" s="2">
+        <v>754</v>
+      </c>
+      <c r="J18" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3.5097399999999999</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2.1581030000000001</v>
+      </c>
+      <c r="I19" s="7">
+        <v>3.820093</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1.815893</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.0758460000000001</v>
+      </c>
+      <c r="I20" s="7">
+        <v>1.2995650000000001</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.51754920000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="2">
+        <v>616</v>
+      </c>
+      <c r="H21" s="2">
+        <v>253</v>
+      </c>
+      <c r="I21" s="7">
+        <v>428</v>
+      </c>
+      <c r="J21" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3.453125</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.3571428999999999</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3.1428571000000001</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3.5097399999999999</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2.1581030000000001</v>
+      </c>
+      <c r="I22" s="2">
+        <v>3.820093</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.827048</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.4972452</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.84309040000000002</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.815893</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1.0758460000000001</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1.2995650000000001</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.51754920000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="2">
+        <v>192</v>
+      </c>
+      <c r="D24" s="2">
+        <v>14</v>
+      </c>
+      <c r="E24" s="2">
+        <v>42</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <v>616</v>
+      </c>
+      <c r="H24" s="2">
+        <v>253</v>
+      </c>
+      <c r="I24" s="2">
+        <v>428</v>
+      </c>
+      <c r="J24" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3.7714289999999999</v>
+      </c>
+      <c r="D25" s="2">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8">
-        <v>0.83349640000000003</v>
-      </c>
-      <c r="F8">
-        <v>1.168798</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9">
-        <v>1680</v>
-      </c>
-      <c r="F9">
-        <v>3140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D16" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="E25" s="2">
+        <v>3.8666670000000001</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2">
+        <v>3.4033739999999999</v>
+      </c>
+      <c r="H25" s="2">
+        <v>2.0751170000000001</v>
+      </c>
+      <c r="I25" s="2">
+        <v>4.0667980000000004</v>
+      </c>
+      <c r="J25" s="2">
+        <v>2.3461539999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2.3167409999999999</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.75377839999999996</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1.1366419999999999</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1.7653920000000001</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1.0297419999999999</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1.427878</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1.281614</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="2">
+        <v>70</v>
+      </c>
+      <c r="D27" s="2">
+        <v>12</v>
+      </c>
+      <c r="E27" s="2">
+        <v>30</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2">
+        <v>652</v>
+      </c>
+      <c r="H27" s="2">
+        <v>213</v>
+      </c>
+      <c r="I27" s="2">
+        <v>509</v>
+      </c>
+      <c r="J27" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3.0159570000000002</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2.0816330000000001</v>
+      </c>
+      <c r="E28" s="2">
+        <v>3.5376340000000002</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1.6666666999999999</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3.1247950000000002</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1.8644069999999999</v>
+      </c>
+      <c r="I28" s="2">
+        <v>3.4905659999999998</v>
+      </c>
+      <c r="J28" s="2">
+        <v>1.2727272999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1.438493</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1.221965</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1.238505</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.81649660000000002</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1.6051500000000001</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1.136504</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1.2592159999999999</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.4670994</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="2">
+        <v>188</v>
+      </c>
+      <c r="D30" s="2">
+        <v>49</v>
+      </c>
+      <c r="E30" s="2">
+        <v>93</v>
+      </c>
+      <c r="F30" s="2">
+        <v>6</v>
+      </c>
+      <c r="G30" s="2">
+        <v>609</v>
+      </c>
+      <c r="H30" s="2">
+        <v>59</v>
+      </c>
+      <c r="I30" s="2">
+        <v>106</v>
+      </c>
+      <c r="J30" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3.0640000000000001</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2.1392410000000002</v>
+      </c>
+      <c r="E31" s="2">
+        <v>3.887324</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2.9363640000000002</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2.0555560000000002</v>
+      </c>
+      <c r="I31" s="2">
+        <v>3.851064</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1.5226459999999999</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1.14056</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1.3426899999999999</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1.447891</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1.172269</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1.367499</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="2">
+        <v>125</v>
+      </c>
+      <c r="D33" s="2">
         <v>79</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
+      <c r="E33" s="2">
+        <v>142</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2">
+        <v>220</v>
+      </c>
+      <c r="H33" s="2">
+        <v>54</v>
+      </c>
+      <c r="I33" s="2">
+        <v>94</v>
+      </c>
+      <c r="J33" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E17" t="s">
+      <c r="C34" s="2">
+        <v>3.5571429999999999</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1.3333333000000001</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2.9333333000000001</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="2">
+        <v>3.875912</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1.625</v>
+      </c>
+      <c r="I34" s="2">
+        <v>2.8064515999999999</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F17" t="s">
+      <c r="C35" s="2">
+        <v>1.8068770000000001</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.57735029999999998</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.96115010000000001</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1.957058</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.80622579999999999</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0.8725195</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="5">
-        <v>3.640523</v>
-      </c>
-      <c r="F18">
+      <c r="C36" s="2">
+        <v>70</v>
+      </c>
+      <c r="D36" s="2">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2">
+        <v>15</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2">
+        <v>137</v>
+      </c>
+      <c r="H36" s="2">
+        <v>16</v>
+      </c>
+      <c r="I36" s="2">
+        <v>31</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" s="2">
+        <v>3.4033739999999999</v>
+      </c>
+      <c r="H37" s="2">
+        <v>2.0751170000000001</v>
+      </c>
+      <c r="I37" s="2">
+        <v>4.0667980000000004</v>
+      </c>
+      <c r="J37" s="2">
+        <v>2.3461539999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38" s="2">
+        <v>1.7653920000000001</v>
+      </c>
+      <c r="H38" s="2">
+        <v>1.0297419999999999</v>
+      </c>
+      <c r="I38" s="2">
+        <v>1.427878</v>
+      </c>
+      <c r="J38" s="2">
+        <v>1.281614</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2">
+        <v>652</v>
+      </c>
+      <c r="H39" s="2">
+        <v>213</v>
+      </c>
+      <c r="I39" s="2">
+        <v>509</v>
+      </c>
+      <c r="J39" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2.5673080000000001</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1.5185869999999999</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.57735029999999998</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0.57735029999999998</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="2">
+        <v>104</v>
+      </c>
+      <c r="D42" s="2">
         <v>4</v>
       </c>
-      <c r="G18">
-        <v>2</v>
+      <c r="E42" s="2">
+        <v>4</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2">
+        <v>3</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D3:G3"/>
+  <mergeCells count="2">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>